<commit_message>
DWH-17: Update Importer tests
</commit_message>
<xml_diff>
--- a/app-importer/src/test/resources/zipcode_locations.xlsx
+++ b/app-importer/src/test/resources/zipcode_locations.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">zipCode</t>
   </si>
   <si>
-    <t xml:space="preserve">lattitude</t>
+    <t xml:space="preserve">latitude</t>
   </si>
   <si>
     <t xml:space="preserve">longitude</t>
@@ -40,10 +40,10 @@
   </numFmts>
   <fonts count="5">
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -65,7 +65,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -77,27 +77,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -126,13 +111,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -152,68 +141,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="18.33"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>456465</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>47.4564697894</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>19.45467878754</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>456466</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="2" t="n">
         <v>47.4564697894</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>19.45467878754</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>